<commit_message>
remove duplicate variable yearly rep urban dict ath_foodenvdens300
</commit_message>
<xml_diff>
--- a/dictionaries/urban_ath/1_3/1_3_yearly_rep.xlsx
+++ b/dictionaries/urban_ath/1_3/1_3_yearly_rep.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PROJECTS\ATHLETE\DOCUMENTS\dictionaries\jose_dictionaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\back\ATHLETE\HARMO\git_hub\dsUploadTest\20240523_uploadurban\dicts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CA1DFD-9D2B-4E74-AF1B-1F0D72003E73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAC9BD1-1055-4F01-8CF3-747289EEEFF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11775" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
     <sheet name="Categories" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$A$1:$D$127</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$A$1:$D$126</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="360">
   <si>
     <t>name</t>
   </si>
@@ -1991,9 +1991,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMH1795"/>
+  <dimension ref="A1:AMH1794"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9330,21 +9332,21 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>189</v>
-      </c>
-      <c r="B86" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B86" t="s">
         <v>20</v>
       </c>
       <c r="C86" t="s">
         <v>114</v>
       </c>
       <c r="D86" t="s">
-        <v>190</v>
+        <v>338</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B87" t="s">
         <v>20</v>
@@ -9353,12 +9355,12 @@
         <v>114</v>
       </c>
       <c r="D87" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B88" t="s">
         <v>20</v>
@@ -9367,12 +9369,12 @@
         <v>114</v>
       </c>
       <c r="D88" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B89" t="s">
         <v>20</v>
@@ -9381,12 +9383,12 @@
         <v>114</v>
       </c>
       <c r="D89" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B90" t="s">
         <v>20</v>
@@ -9395,12 +9397,12 @@
         <v>114</v>
       </c>
       <c r="D90" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B91" t="s">
         <v>20</v>
@@ -9409,12 +9411,12 @@
         <v>114</v>
       </c>
       <c r="D91" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B92" t="s">
         <v>20</v>
@@ -9423,12 +9425,12 @@
         <v>114</v>
       </c>
       <c r="D92" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B93" t="s">
         <v>20</v>
@@ -9437,12 +9439,12 @@
         <v>114</v>
       </c>
       <c r="D93" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B94" t="s">
         <v>20</v>
@@ -9451,12 +9453,12 @@
         <v>114</v>
       </c>
       <c r="D94" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B95" t="s">
         <v>20</v>
@@ -9465,12 +9467,12 @@
         <v>114</v>
       </c>
       <c r="D95" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B96" t="s">
         <v>20</v>
@@ -9479,12 +9481,12 @@
         <v>114</v>
       </c>
       <c r="D96" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B97" t="s">
         <v>20</v>
@@ -9493,12 +9495,12 @@
         <v>114</v>
       </c>
       <c r="D97" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B98" t="s">
         <v>20</v>
@@ -9507,12 +9509,12 @@
         <v>114</v>
       </c>
       <c r="D98" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B99" t="s">
         <v>20</v>
@@ -9521,12 +9523,12 @@
         <v>114</v>
       </c>
       <c r="D99" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B100" t="s">
         <v>20</v>
@@ -9535,12 +9537,12 @@
         <v>114</v>
       </c>
       <c r="D100" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B101" t="s">
         <v>20</v>
@@ -9549,12 +9551,12 @@
         <v>114</v>
       </c>
       <c r="D101" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B102" t="s">
         <v>20</v>
@@ -9563,12 +9565,12 @@
         <v>114</v>
       </c>
       <c r="D102" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B103" t="s">
         <v>20</v>
@@ -9577,12 +9579,12 @@
         <v>114</v>
       </c>
       <c r="D103" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B104" t="s">
         <v>20</v>
@@ -9591,12 +9593,12 @@
         <v>114</v>
       </c>
       <c r="D104" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B105" t="s">
         <v>20</v>
@@ -9605,12 +9607,12 @@
         <v>114</v>
       </c>
       <c r="D105" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B106" t="s">
         <v>20</v>
@@ -9619,12 +9621,12 @@
         <v>114</v>
       </c>
       <c r="D106" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B107" t="s">
         <v>20</v>
@@ -9633,26 +9635,26 @@
         <v>114</v>
       </c>
       <c r="D107" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>337</v>
+        <v>191</v>
       </c>
       <c r="B108" t="s">
         <v>20</v>
       </c>
-      <c r="C108" t="s">
-        <v>114</v>
+      <c r="C108" s="5" t="s">
+        <v>192</v>
       </c>
       <c r="D108" t="s">
-        <v>359</v>
+        <v>193</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B109" t="s">
         <v>20</v>
@@ -9661,12 +9663,12 @@
         <v>192</v>
       </c>
       <c r="D109" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B110" t="s">
         <v>20</v>
@@ -9675,26 +9677,26 @@
         <v>192</v>
       </c>
       <c r="D110" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B111" t="s">
         <v>20</v>
       </c>
-      <c r="C111" s="5" t="s">
-        <v>192</v>
+      <c r="C111" t="s">
+        <v>99</v>
       </c>
       <c r="D111" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B112" t="s">
         <v>20</v>
@@ -9703,12 +9705,12 @@
         <v>99</v>
       </c>
       <c r="D112" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B113" t="s">
         <v>20</v>
@@ -9717,26 +9719,26 @@
         <v>99</v>
       </c>
       <c r="D113" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B114" t="s">
         <v>20</v>
       </c>
-      <c r="C114" t="s">
-        <v>99</v>
+      <c r="C114" s="5" t="s">
+        <v>192</v>
       </c>
       <c r="D114" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B115" t="s">
         <v>20</v>
@@ -9745,12 +9747,12 @@
         <v>192</v>
       </c>
       <c r="D115" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B116" t="s">
         <v>20</v>
@@ -9759,82 +9761,82 @@
         <v>192</v>
       </c>
       <c r="D116" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B117" t="s">
         <v>20</v>
       </c>
-      <c r="C117" s="5" t="s">
-        <v>192</v>
+      <c r="C117" t="s">
+        <v>99</v>
       </c>
       <c r="D117" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B118" t="s">
         <v>20</v>
       </c>
-      <c r="C118" t="s">
-        <v>99</v>
+      <c r="C118" s="5" t="s">
+        <v>213</v>
       </c>
       <c r="D118" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B119" t="s">
         <v>20</v>
       </c>
-      <c r="C119" s="5" t="s">
-        <v>213</v>
+      <c r="C119" t="s">
+        <v>216</v>
       </c>
       <c r="D119" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B120" t="s">
         <v>20</v>
       </c>
       <c r="C120" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D120" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B121" t="s">
         <v>20</v>
       </c>
-      <c r="C121" t="s">
-        <v>219</v>
+      <c r="C121" s="5" t="s">
+        <v>222</v>
       </c>
       <c r="D121" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B122" t="s">
         <v>20</v>
@@ -9843,12 +9845,12 @@
         <v>222</v>
       </c>
       <c r="D122" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B123" t="s">
         <v>20</v>
@@ -9857,69 +9859,61 @@
         <v>222</v>
       </c>
       <c r="D123" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B124" t="s">
         <v>20</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>222</v>
+        <v>192</v>
       </c>
       <c r="D124" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B125" t="s">
         <v>20</v>
       </c>
-      <c r="C125" s="5" t="s">
-        <v>192</v>
+      <c r="C125" t="s">
+        <v>72</v>
       </c>
       <c r="D125" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B126" t="s">
         <v>20</v>
       </c>
-      <c r="C126" t="s">
-        <v>72</v>
+      <c r="C126" s="5" t="s">
+        <v>233</v>
       </c>
       <c r="D126" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
-        <v>232</v>
-      </c>
-      <c r="B127" t="s">
-        <v>20</v>
-      </c>
-      <c r="C127" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="D127" t="s">
-        <v>234</v>
-      </c>
+      <c r="A127"/>
+      <c r="B127"/>
+      <c r="C127" s="5"/>
+      <c r="D127"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128"/>
       <c r="B128"/>
-      <c r="C128" s="5"/>
+      <c r="C128"/>
       <c r="D128"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
@@ -10385,9 +10379,6 @@
       <c r="D205"/>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A206"/>
-      <c r="B206"/>
-      <c r="C206"/>
       <c r="D206"/>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
@@ -15154,13 +15145,10 @@
     <row r="1794" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D1794"/>
     </row>
-    <row r="1795" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D1795"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D127" xr:uid="{AF393D00-D786-4826-A0C4-1A75D9C3171B}"/>
+  <autoFilter ref="A1:D126" xr:uid="{AF393D00-D786-4826-A0C4-1A75D9C3171B}"/>
   <dataValidations count="1">
-    <dataValidation type="list" showErrorMessage="1" sqref="C7:C37 C128 C125 B4:B85 C44:C85 C109:C122 B87:B213" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" showErrorMessage="1" sqref="C7:C37 C127 C124 B4:B85 C44:C85 C108:C121 B86:B212" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"integer,decimal,text,binary,locale,boolean,datetime,date"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>